<commit_message>
excel api status updated
</commit_message>
<xml_diff>
--- a/API_status.xlsx
+++ b/API_status.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luigizurlo/Desktop/skills-matrix/skills-matrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D6FC66-1069-2546-AC05-B58192618270}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECA895F-18AB-8D4C-B876-2493692CDFFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{ECE6D8FE-F0AA-1C44-A28F-3105C4403852}"/>
+    <workbookView xWindow="28980" yWindow="1280" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{ECE6D8FE-F0AA-1C44-A28F-3105C4403852}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Refactoring" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="55">
   <si>
     <t>API</t>
   </si>
@@ -165,12 +166,6 @@
     <t>dir missing</t>
   </si>
   <si>
-    <t>ERR</t>
-  </si>
-  <si>
-    <t>query error: skill.display_name does not exist</t>
-  </si>
-  <si>
     <t>SERVICES:</t>
   </si>
   <si>
@@ -184,6 +179,24 @@
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>TODO(ok)</t>
+  </si>
+  <si>
+    <t>dir missing -&gt; created</t>
+  </si>
+  <si>
+    <t>TODO(ok):</t>
+  </si>
+  <si>
+    <t>pr</t>
+  </si>
+  <si>
+    <t>also private apis</t>
+  </si>
+  <si>
+    <t>Update team --&gt; project???</t>
   </si>
 </sst>
 </file>
@@ -255,7 +268,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -304,6 +317,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -505,7 +524,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -566,6 +585,10 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -891,7 +914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81843F32-1920-9C4B-9934-F53A923D3181}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -955,7 +978,7 @@
       </c>
       <c r="C3" s="10"/>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -966,17 +989,17 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="21">
@@ -988,7 +1011,7 @@
       </c>
       <c r="C5" s="10"/>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -1022,22 +1045,22 @@
         <v>9</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I6" s="28">
-        <f>COUNTIF(B2:B35,"OK") + COUNTIF(B2:B35,"TODO") + COUNTIF(B2:B35,"ERR")</f>
+        <f>COUNTIF(B2:B35,"OK") + COUNTIF(B2:B35,"TODO") + COUNTIF(B2:B35,"TODO(ok)")</f>
         <v>34</v>
       </c>
       <c r="J6" s="28">
-        <f>COUNTIF(C2:C35,"OK") + COUNTIF(C2:C35,"TODO") + COUNTIF(C2:C35,"ERR")</f>
+        <f>COUNTIF(C2:C35,"OK") + COUNTIF(C2:C35,"TODO") + COUNTIF(C2:C35,"TODO(ok)")</f>
         <v>11</v>
       </c>
       <c r="K6" s="28">
-        <f>COUNTIF(D2:D35,"OK") + COUNTIF(D2:D35,"TODO") + COUNTIF(D2:D35,"ERR")</f>
+        <f>COUNTIF(D2:D35,"OK") + COUNTIF(D2:D35,"TODO") + COUNTIF(D2:D35,"TODO(ok)")</f>
         <v>10</v>
       </c>
       <c r="L6" s="29">
-        <f>COUNTIF(E2:E35,"OK") + COUNTIF(E2:E35,"TODO") + COUNTIF(E2:E35,"ERR")</f>
+        <f>COUNTIF(E2:E35,"OK") + COUNTIF(E2:E35,"TODO") + COUNTIF(E2:E35,"TODO(ok)")</f>
         <v>16</v>
       </c>
     </row>
@@ -1050,17 +1073,17 @@
       </c>
       <c r="C7" s="10"/>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I7" s="24">
         <f>COUNTIF(B2:B35,"OK")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J7" s="24">
         <f>COUNTIF(C2:C35,"OK")</f>
@@ -1080,7 +1103,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -1088,19 +1111,19 @@
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="H8" s="32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I8" s="24">
         <f>COUNTIF(B2:B35,"TODO")</f>
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="J8" s="24">
         <f>COUNTIF(C2:C35,"TODO")</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K8" s="24">
         <f>COUNTIF(D2:D35,"TODO")</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L8" s="25">
         <f>COUNTIF(E2:E35,"TODO")</f>
@@ -1120,22 +1143,22 @@
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="H9" s="33" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I9" s="26">
-        <f>COUNTIF(B2:B35,"ERR")</f>
+        <f>COUNTIF(B2:B35,"TODO(ok)")</f>
+        <v>5</v>
+      </c>
+      <c r="J9" s="26">
+        <f>COUNTIF(C2:C35,"TODO(ok)")</f>
         <v>1</v>
       </c>
-      <c r="J9" s="26">
-        <f>COUNTIF(C2:C35,"ERR")</f>
-        <v>0</v>
-      </c>
       <c r="K9" s="26">
-        <f>COUNTIF(D2:D35,"ERR")</f>
-        <v>0</v>
+        <f>COUNTIF(D2:D35,"TODO(ok)")</f>
+        <v>8</v>
       </c>
       <c r="L9" s="27">
-        <f>COUNTIF(E2:E35,"ERR")</f>
+        <f>COUNTIF(E2:E35,"TODO(ok)")</f>
         <v>0</v>
       </c>
     </row>
@@ -1148,7 +1171,7 @@
       </c>
       <c r="C10" s="10"/>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -1174,17 +1197,17 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="H12" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I12" s="14">
         <f>COUNTIF(B2:E35,"OK") + COUNTIF(B2:E35,"TODO") + COUNTIF(B2:E35,"ERR")</f>
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1192,7 +1215,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -1202,11 +1225,11 @@
         <v>9</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I13" s="16">
         <f>COUNTIF(B2:E35,"OK")</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1217,18 +1240,18 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" t="s">
         <v>9</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I14" s="16">
         <f>COUNTIF(B2:E35,"TODO")</f>
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="20" thickBot="1">
@@ -1242,11 +1265,11 @@
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="H15" s="17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I15" s="18">
         <f>COUNTIF(B2:E35,"ERR")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1303,6 +1326,10 @@
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
+      <c r="H20">
+        <f>COUNTIF(B2:E35,"TODO(ok)")</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
@@ -1414,7 +1441,7 @@
       </c>
       <c r="C29" s="10"/>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="E29" t="s">
         <v>9</v>
@@ -1440,7 +1467,7 @@
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
         <v>9</v>
@@ -1448,9 +1475,6 @@
       <c r="D31" s="10"/>
       <c r="E31" t="s">
         <v>9</v>
-      </c>
-      <c r="F31" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1458,7 +1482,7 @@
         <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -1488,7 +1512,7 @@
       </c>
       <c r="C34" s="10"/>
       <c r="D34" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="E34" t="s">
         <v>7</v>
@@ -1503,7 +1527,7 @@
       </c>
       <c r="C35" s="10"/>
       <c r="D35" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="E35" t="s">
         <v>7</v>
@@ -1518,4 +1542,652 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5BE8F5C-587A-6F4A-85A1-D70D17911ABC}">
+  <dimension ref="A1:L35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <cols>
+    <col min="1" max="1" width="52" style="3" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="24">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="36" customFormat="1">
+      <c r="A3" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="35"/>
+    </row>
+    <row r="4" spans="1:12" s="36" customFormat="1" ht="20" thickBot="1">
+      <c r="A4" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="21">
+      <c r="A5" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="35"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="35"/>
+      <c r="H6" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="28">
+        <f>COUNTIF(B2:B35,"OK") + COUNTIF(B2:B35,"TODO") + COUNTIF(B2:B35,"TODO(ok)")</f>
+        <v>34</v>
+      </c>
+      <c r="J6" s="28">
+        <f>COUNTIF(C2:C35,"OK") + COUNTIF(C2:C35,"TODO") + COUNTIF(C2:C35,"TODO(ok)")</f>
+        <v>11</v>
+      </c>
+      <c r="K6" s="28">
+        <f>COUNTIF(D2:D35,"OK") + COUNTIF(D2:D35,"TODO") + COUNTIF(D2:D35,"TODO(ok)")</f>
+        <v>10</v>
+      </c>
+      <c r="L6" s="29">
+        <f>COUNTIF(E2:E35,"OK") + COUNTIF(E2:E35,"TODO") + COUNTIF(E2:E35,"TODO(ok)")</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="35"/>
+      <c r="H7" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="24">
+        <f>COUNTIF(B2:B35,"OK")</f>
+        <v>18</v>
+      </c>
+      <c r="J7" s="24">
+        <f>COUNTIF(C2:C35,"OK")</f>
+        <v>9</v>
+      </c>
+      <c r="K7" s="24">
+        <f>COUNTIF(D2:D35,"OK")</f>
+        <v>8</v>
+      </c>
+      <c r="L7" s="25">
+        <f>COUNTIF(E2:E35,"OK")</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="H8" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="24">
+        <f>COUNTIF(B2:B35,"TODO")</f>
+        <v>16</v>
+      </c>
+      <c r="J8" s="24">
+        <f>COUNTIF(C2:C35,"TODO")</f>
+        <v>2</v>
+      </c>
+      <c r="K8" s="24">
+        <f>COUNTIF(D2:D35,"TODO")</f>
+        <v>2</v>
+      </c>
+      <c r="L8" s="25">
+        <f>COUNTIF(E2:E35,"TODO")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="20" thickBot="1">
+      <c r="A9" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="H9" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="26">
+        <f>COUNTIF(B2:B35,"TODO(ok)")</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="26">
+        <f>COUNTIF(C2:C35,"TODO(ok)")</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="26">
+        <f>COUNTIF(D2:D35,"TODO(ok)")</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="27">
+        <f>COUNTIF(E2:E35,"TODO(ok)")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="35"/>
+    </row>
+    <row r="11" spans="1:12" ht="20" thickBot="1">
+      <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="H12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="14">
+        <f>COUNTIF(B2:E35,"OK") + COUNTIF(B2:E35,"TODO") + COUNTIF(B2:E35,"ERR")</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="35"/>
+      <c r="H13" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="16">
+        <f>COUNTIF(B2:E35,"OK")</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="35"/>
+      <c r="H14" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="16">
+        <f>COUNTIF(B2:E35,"TODO")</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="20" thickBot="1">
+      <c r="A15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="H15" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="18">
+        <f>COUNTIF(B2:E35,"ERR")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="35"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="35"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="35"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H1" r:id="rId1" xr:uid="{D9BEDC4A-6343-F74C-9BF9-31A8766752C1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>